<commit_message>
continue PyInputPlus To Do: input validation (isalpha)
</commit_message>
<xml_diff>
--- a/DustBusters/add_data.xlsx
+++ b/DustBusters/add_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yello\Documents\GitHub\SheCodes\DustBusters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DDD6E8-408E-4CA4-B2B9-CCEF27BB1F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D973876-8821-4AC5-8BAC-860D3C5E68D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>General Manager</t>
   </si>
   <si>
-    <t>Martin Zess</t>
-  </si>
-  <si>
     <t>Coordinator</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>Python, JavaScript</t>
+  </si>
+  <si>
+    <t>Mark Zess</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -424,10 +424,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -444,7 +444,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -452,16 +452,16 @@
         <v>443346</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>